<commit_message>
README and Documentation tidy up.
</commit_message>
<xml_diff>
--- a/Documentation/Data Vault - Northwind.xlsx
+++ b/Documentation/Data Vault - Northwind.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db8d30ba3537acd5/Data Engineering/Data Vault/Data-Vault-Example-Northwind/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1104" documentId="13_ncr:1_{DD5DDCC3-190E-4B47-8546-EDFD77CA3992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A3F8E87-3FC8-4A67-98DD-0B9E42DB0356}"/>
+  <xr:revisionPtr revIDLastSave="1149" documentId="13_ncr:1_{DD5DDCC3-190E-4B47-8546-EDFD77CA3992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD4B5047-E92E-4164-96B6-2712EB0ADA6C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6207AA47-5294-48E0-8A61-6F3DBD8121A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{6207AA47-5294-48E0-8A61-6F3DBD8121A6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Models" sheetId="2" r:id="rId1"/>
+    <sheet name="Data Modelling" sheetId="2" r:id="rId1"/>
     <sheet name="Database Summary" sheetId="11" r:id="rId2"/>
     <sheet name="Table Mapping" sheetId="9" r:id="rId3"/>
-    <sheet name="Notes" sheetId="10" r:id="rId4"/>
+    <sheet name="Rules + Conventions" sheetId="10" r:id="rId4"/>
+    <sheet name="Notes" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="221">
   <si>
     <t>Categories</t>
   </si>
@@ -675,6 +676,33 @@
   <si>
     <t>Sourced from the Data Vault database, the Information Mart is intended for access by end users for analysis. Data is modelled as star schema. 
 I have also included 'replica' views just to help illustrate how source data can be accurately replicated from Data Vault tables.</t>
+  </si>
+  <si>
+    <t>My implementation here most closely adheres to Dan Linstedt's Data Vault 2.0 standard, but also takes some inspiration from the work of others, primarily Hans Hultgren and Patrick Cuba.</t>
+  </si>
+  <si>
+    <t>This implementation should not be considered 'textbook' or representative of a real production Data Vault data warehouse; it is intended as a simplified example for educational purposes. A full-scale production data warehouse would almost certainly integrate data from multiple source systems, use incremental loads, and employ parallelised ETL scheduling as a just a few examples. My goal here was to have something somebody can set up, load, and be getting info out of the information mart with just SQL Server in a matter of minutes.</t>
+  </si>
+  <si>
+    <t>My approach to Satellite types is simplistic, illustrating a few basic functions they commonly serve - link effectivity (including deletions and driving key relationships), business key deletions, and historisation of contextual attributes.</t>
+  </si>
+  <si>
+    <t>This project was coded by hand, so no doubt there are a few inconsistencies in coding conventions. In a professional Data Vault implementation, I would consider a code automation tool to be a non-negotiable expense (WhereScape 3D/RED, Vaultspeed, dbtvault, etc.).</t>
+  </si>
+  <si>
+    <t>Business keys in Northwind are seldom uniquely indexed, so the surrogate IDs have been used where necessary.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information Mart objects are fully virtual, i.e. views. In addition to star schema facts, dimensions, and bridges, I have included 'replica' views, which, as the name suggests, exactly replicate all Northwind database source tables from their respective Data Vault objects. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information Mart views present 'current' data as it existed in the data warehouse as at the specific (load effective) time specified in the 'Value' field of the 'Information_Mart_Load_Effective_Datetime' (ID = 1) record in Meta_Metrics_Error_Mart.meta.Parameter. If this field is left blank, the current datetime will be employed. This functionality is enabled by the use of PIT tables built for each Hub. </t>
+  </si>
+  <si>
+    <t>Remaining to-do items include fleshing out the Meta_Metrics_Error_Mart and tweaking indexing for Information_Mart query performance.</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -960,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -970,9 +998,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1001,9 +1026,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -1015,9 +1037,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1036,27 +1055,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1066,6 +1064,31 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1161,7 +1184,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>390698</xdr:colOff>
+      <xdr:colOff>417592</xdr:colOff>
       <xdr:row>91</xdr:row>
       <xdr:rowOff>159677</xdr:rowOff>
     </xdr:to>
@@ -1608,13 +1631,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1F2E83-6FDB-4A03-B328-43C2FD5404DD}">
   <dimension ref="B2:C96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView showGridLines="0" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="25.8" x14ac:dyDescent="0.5">
@@ -1628,18 +1651,18 @@
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="61"/>
+      <c r="B47" s="58"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="61"/>
-      <c r="C48" s="62"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="59"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="61"/>
-      <c r="C49" s="62"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="59"/>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C94" s="62"/>
+      <c r="C94" s="59"/>
     </row>
     <row r="96" spans="2:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B96" s="2" t="s">
@@ -1665,7 +1688,7 @@
   <cols>
     <col min="1" max="1" width="3.77734375" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="107" style="71" customWidth="1"/>
+    <col min="3" max="3" width="107" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="25.8" x14ac:dyDescent="0.5">
@@ -1674,50 +1697,50 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="63" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="61" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="61" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="61" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="62" t="s">
         <v>205</v>
       </c>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="61" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="61" t="s">
         <v>211</v>
       </c>
     </row>
@@ -1728,15 +1751,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7052CFE6-7CEF-4EA6-9632-54441F5C923E}">
-  <dimension ref="B2:Q42"/>
+  <dimension ref="A2:Q42"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
@@ -1754,20 +1777,20 @@
     <col min="17" max="17" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E2" s="60"/>
-    </row>
-    <row r="3" spans="2:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="E2" s="57"/>
+    </row>
+    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="47" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="45" t="s">
         <v>157</v>
       </c>
       <c r="D4" s="64" t="s">
@@ -1791,1009 +1814,1010 @@
       <c r="P4" s="64"/>
       <c r="Q4" s="64"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="48" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="67"/>
+      <c r="B5" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68" t="s">
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="36" t="s">
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="69" t="s">
         <v>141</v>
       </c>
-      <c r="O5" s="63" t="s">
+      <c r="O5" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="49" t="s">
+      <c r="P5" s="71"/>
+      <c r="Q5" s="71"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="N6" s="56" t="s">
+      <c r="N6" s="53" t="s">
         <v>175</v>
       </c>
-      <c r="O6" s="37" t="s">
+      <c r="O6" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="P6" s="37" t="s">
+      <c r="P6" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="Q6" s="37" t="s">
+      <c r="Q6" s="35" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="50" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="55" t="s">
+      <c r="E7" s="19"/>
+      <c r="F7" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="30" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="38" t="s">
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39" t="s">
+      <c r="O7" s="37"/>
+      <c r="P7" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="Q7" s="39"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23" t="s">
+      <c r="Q7" s="37"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="48"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="32" t="s">
+      <c r="G8" s="23"/>
+      <c r="H8" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="52" t="s">
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="34" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="43" t="s">
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="O9" s="44"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45" t="s">
+      <c r="O9" s="42"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="53" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20" t="s">
+      <c r="E10" s="19"/>
+      <c r="F10" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="30" t="s">
+      <c r="G10" s="20"/>
+      <c r="H10" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="46" t="s">
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39" t="s">
+      <c r="O10" s="37"/>
+      <c r="P10" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="Q10" s="39"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="51"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23" t="s">
+      <c r="Q10" s="37"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="48"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="32" t="s">
+      <c r="G11" s="23"/>
+      <c r="H11" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="50" t="s">
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="30" t="s">
+      <c r="G12" s="20"/>
+      <c r="H12" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="I12" s="30" t="s">
+      <c r="I12" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="38" t="s">
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39" t="s">
+      <c r="O12" s="37"/>
+      <c r="P12" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="Q12" s="39"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="51"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23" t="s">
+      <c r="Q12" s="37"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="48"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="32" t="s">
+      <c r="G13" s="23"/>
+      <c r="H13" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="53" t="s">
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="30" t="s">
+      <c r="G14" s="20"/>
+      <c r="H14" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="46" t="s">
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39" t="s">
+      <c r="O14" s="37"/>
+      <c r="P14" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="Q14" s="39"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="53"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20" t="s">
+      <c r="Q14" s="37"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="50"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="30" t="s">
+      <c r="G15" s="20"/>
+      <c r="H15" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39" t="s">
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="Q15" s="39"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23" t="s">
+      <c r="Q15" s="37"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="48"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="32" t="s">
+      <c r="G16" s="23"/>
+      <c r="H16" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="34" t="s">
+      <c r="G17" s="26"/>
+      <c r="H17" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="43" t="s">
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="O17" s="44"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45" t="s">
+      <c r="O17" s="42"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="30" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="30" t="s">
+      <c r="J18" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="K18" s="30" t="s">
+      <c r="K18" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="L18" s="30" t="s">
+      <c r="L18" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="M18" s="31"/>
-      <c r="N18" s="46" t="s">
+      <c r="M18" s="30"/>
+      <c r="N18" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="O18" s="39" t="s">
+      <c r="O18" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="51"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23" t="s">
+      <c r="B19" s="48"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="32" t="s">
+      <c r="G19" s="23"/>
+      <c r="H19" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="30" t="s">
+      <c r="G20" s="20"/>
+      <c r="H20" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="I20" s="30" t="s">
+      <c r="I20" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="J20" s="30" t="s">
+      <c r="J20" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="K20" s="30" t="s">
+      <c r="K20" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="L20" s="30" t="s">
+      <c r="L20" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="M20" s="31"/>
-      <c r="N20" s="46" t="s">
+      <c r="M20" s="30"/>
+      <c r="N20" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="O20" s="39" t="s">
+      <c r="O20" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B21" s="53"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20" t="s">
+      <c r="B21" s="50"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="G21" s="21"/>
-      <c r="H21" s="30" t="s">
+      <c r="G21" s="20"/>
+      <c r="H21" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30" t="s">
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="L21" s="30" t="s">
+      <c r="L21" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="M21" s="31"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="39" t="s">
+      <c r="M21" s="30"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B22" s="51"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23" t="s">
+      <c r="B22" s="48"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="32" t="s">
+      <c r="G22" s="23"/>
+      <c r="H22" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="30" t="s">
+      <c r="G23" s="20"/>
+      <c r="H23" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="J23" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="46" t="s">
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39" t="s">
+      <c r="O23" s="37"/>
+      <c r="P23" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="Q23" s="39"/>
+      <c r="Q23" s="37"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B24" s="53"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20" t="s">
+      <c r="B24" s="50"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="30" t="s">
+      <c r="G24" s="20"/>
+      <c r="H24" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="39"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B25" s="53"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20" t="s">
+      <c r="B25" s="50"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="30" t="s">
+      <c r="G25" s="20"/>
+      <c r="H25" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="39"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B26" s="51"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23" t="s">
+      <c r="B26" s="48"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="32" t="s">
+      <c r="G26" s="23"/>
+      <c r="H26" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="40"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20" t="s">
+      <c r="E27" s="19"/>
+      <c r="F27" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="21"/>
-      <c r="H27" s="30" t="s">
+      <c r="G27" s="20"/>
+      <c r="H27" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="I27" s="30" t="s">
+      <c r="I27" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="J27" s="30" t="s">
+      <c r="J27" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="46" t="s">
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="O27" s="39"/>
-      <c r="P27" s="39" t="s">
+      <c r="O27" s="37"/>
+      <c r="P27" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="Q27" s="39"/>
+      <c r="Q27" s="37"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B28" s="51"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23" t="s">
+      <c r="B28" s="48"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="32" t="s">
+      <c r="G28" s="23"/>
+      <c r="H28" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B29" s="53" t="s">
+      <c r="B29" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20" t="s">
+      <c r="E29" s="19"/>
+      <c r="F29" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="21"/>
-      <c r="H29" s="30" t="s">
+      <c r="G29" s="20"/>
+      <c r="H29" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="I29" s="30" t="s">
+      <c r="I29" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="J29" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="46" t="s">
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39" t="s">
+      <c r="O29" s="37"/>
+      <c r="P29" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="Q29" s="39"/>
+      <c r="Q29" s="37"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B30" s="51"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23" t="s">
+      <c r="B30" s="48"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="24"/>
-      <c r="H30" s="32" t="s">
+      <c r="G30" s="23"/>
+      <c r="H30" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20" t="s">
+      <c r="E31" s="19"/>
+      <c r="F31" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="30" t="s">
+      <c r="G31" s="20"/>
+      <c r="H31" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="J31" s="30" t="s">
+      <c r="J31" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="46" t="s">
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39" t="s">
+      <c r="O31" s="37"/>
+      <c r="P31" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="Q31" s="39"/>
+      <c r="Q31" s="37"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B32" s="51"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23" t="s">
+      <c r="B32" s="48"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G32" s="24"/>
-      <c r="H32" s="32" t="s">
+      <c r="G32" s="23"/>
+      <c r="H32" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="40"/>
-      <c r="O32" s="41"/>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="40"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G33" s="21"/>
-      <c r="H33" s="30" t="s">
+      <c r="G33" s="20"/>
+      <c r="H33" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="I33" s="30" t="s">
+      <c r="I33" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="J33" s="30" t="s">
+      <c r="J33" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="38" t="s">
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="O33" s="39"/>
-      <c r="P33" s="39" t="s">
+      <c r="O33" s="37"/>
+      <c r="P33" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="Q33" s="39"/>
+      <c r="Q33" s="37"/>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B34" s="53"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20" t="s">
+      <c r="B34" s="50"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="21"/>
-      <c r="H34" s="30" t="s">
+      <c r="G34" s="20"/>
+      <c r="H34" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="46"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="39"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="37"/>
+      <c r="P34" s="37"/>
+      <c r="Q34" s="37"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B35" s="51"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23" t="s">
+      <c r="B35" s="48"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="32" t="s">
+      <c r="G35" s="23"/>
+      <c r="H35" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="54"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="42"/>
-      <c r="Q35" s="42"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="40"/>
+      <c r="Q35" s="40"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B36" s="50"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="58" t="s">
+      <c r="B36" s="47"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="55" t="s">
         <v>165</v>
       </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="57" t="s">
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="N36" s="38"/>
-      <c r="O36" s="39"/>
-      <c r="P36" s="39" t="s">
+      <c r="N36" s="36"/>
+      <c r="O36" s="37"/>
+      <c r="P36" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="Q36" s="39"/>
+      <c r="Q36" s="37"/>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B37" s="53"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="31"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="39"/>
-      <c r="P37" s="39" t="s">
+      <c r="B37" s="50"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="Q37" s="39"/>
+      <c r="Q37" s="37"/>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B38" s="53"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="46"/>
-      <c r="O38" s="39"/>
-      <c r="P38" s="39" t="s">
+      <c r="B38" s="50"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="Q38" s="39"/>
+      <c r="Q38" s="37"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B39" s="53"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="31"/>
-      <c r="N39" s="46"/>
-      <c r="O39" s="39"/>
-      <c r="P39" s="39" t="s">
+      <c r="B39" s="50"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="Q39" s="39"/>
+      <c r="Q39" s="37"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C42" s="8"/>
@@ -2828,143 +2852,280 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A415F46-8E07-4FE7-966B-4E63E945769C}">
-  <dimension ref="A2:C21"/>
+  <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="45.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="2:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B2" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A19" s="2" t="s">
+    <row r="18" spans="2:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B18" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="61"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="61"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="61"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="61"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="61"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="61"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="61"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="61"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="61"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="61"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="61"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="61"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="61"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="61"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="61"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EB0B39-FEE6-4851-B80D-8D7DB2E66E7B}">
+  <dimension ref="B2:B18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="128.77734375" style="62" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="65" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="66" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="66"/>
+    </row>
+    <row r="6" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="66" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="66"/>
+    </row>
+    <row r="8" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="66" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="66"/>
+    </row>
+    <row r="10" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="66" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="66"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="66" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="66"/>
+    </row>
+    <row r="14" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="66" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="66"/>
+    </row>
+    <row r="16" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="66" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="66"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="66" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>